<commit_message>
Direct To You script updated: shipping validations
</commit_message>
<xml_diff>
--- a/KatalonProjects/virtualShowData.xlsx
+++ b/KatalonProjects/virtualShowData.xlsx
@@ -516,10 +516,10 @@
         <v>23</v>
       </c>
       <c r="K2">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="L2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M2">
         <v>2019</v>

</xml_diff>